<commit_message>
improved to book a waybill thru waybill sheet with dims
</commit_message>
<xml_diff>
--- a/backend/shipping/data/success.xlsx
+++ b/backend/shipping/data/success.xlsx
@@ -23,13 +23,13 @@
     <t>Date</t>
   </si>
   <si>
-    <t>77707349661</t>
+    <t>77707349716</t>
   </si>
   <si>
-    <t>CR940111</t>
+    <t>CR940116</t>
   </si>
   <si>
-    <t>2026-02-03T07:10:52.846504044</t>
+    <t>2026-02-03T07:39:49.353376525</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
added bulk dimentions in excel upload
</commit_message>
<xml_diff>
--- a/backend/shipping/data/success.xlsx
+++ b/backend/shipping/data/success.xlsx
@@ -23,13 +23,13 @@
     <t>Date</t>
   </si>
   <si>
-    <t>77707349716</t>
+    <t>77707349731</t>
   </si>
   <si>
-    <t>CR940116</t>
+    <t>CR940118</t>
   </si>
   <si>
-    <t>2026-02-03T07:39:49.353376525</t>
+    <t>2026-02-03T08:40:11.131594984</t>
   </si>
 </sst>
 </file>

</xml_diff>